<commit_message>
Neuer commit zum zeigen
</commit_message>
<xml_diff>
--- a/Data/Downloads/List of emerging and developing countries.xlsx
+++ b/Data/Downloads/List of emerging and developing countries.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10510"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10614"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/timodaehler/Desktop/Dropbox/COVID19DEBT/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/timodaehler/Desktop/COVID19-DOMINANCE/Data/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D5D07456-A018-D741-9642-DD8AEDCD5C22}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14438889-051A-2C46-AD99-03D1993F54C5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" xr2:uid="{7C8B2377-A4E9-FA4D-B16E-B5B4E93033BD}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="16000" activeTab="1" xr2:uid="{7C8B2377-A4E9-FA4D-B16E-B5B4E93033BD}"/>
   </bookViews>
   <sheets>
     <sheet name="COMPARISON" sheetId="3" r:id="rId1"/>
     <sheet name="IMF" sheetId="1" r:id="rId2"/>
     <sheet name="WORLD BANK" sheetId="2" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -1108,8 +1108,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F51BBD26-1486-6E48-BAF9-1E43B3D5D876}">
   <dimension ref="A1:D165"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -3051,8 +3051,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F25E8A50-35DE-9E4C-9926-61D8832B686D}">
   <dimension ref="A1:H159"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5:A159"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>

</xml_diff>